<commit_message>
Build Client Hello message
</commit_message>
<xml_diff>
--- a/Protocolo.xlsx
+++ b/Protocolo.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>FF</t>
   </si>
@@ -102,18 +102,6 @@
   </si>
   <si>
     <t>TODO: Add shared network key</t>
-  </si>
-  <si>
-    <t>Nodo</t>
-  </si>
-  <si>
-    <t>MAC</t>
-  </si>
-  <si>
-    <t>NodeId</t>
-  </si>
-  <si>
-    <t>Key</t>
   </si>
 </sst>
 </file>
@@ -1002,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R18"/>
+  <dimension ref="B2:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1019,12 +1007,12 @@
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1032,12 +1020,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1072,7 +1060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -1089,7 +1077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1106,12 +1094,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1128,35 +1116,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="O13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13">
-        <v>6</v>
-      </c>
-      <c r="Q13">
-        <v>2</v>
-      </c>
-      <c r="R13">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P14" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>29</v>
-      </c>
-      <c r="R14" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G15" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Gateway receives DH1 message
</commit_message>
<xml_diff>
--- a/Protocolo.xlsx
+++ b/Protocolo.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>FF</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>TODO: Add shared network key</t>
+  </si>
+  <si>
+    <t>Nodo</t>
+  </si>
+  <si>
+    <t>MAC</t>
+  </si>
+  <si>
+    <t>NodeId</t>
+  </si>
+  <si>
+    <t>Key</t>
   </si>
 </sst>
 </file>
@@ -990,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K18"/>
+  <dimension ref="B2:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1007,12 +1019,12 @@
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1020,12 +1032,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -1042,7 +1054,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1060,7 +1072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -1077,7 +1089,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1094,12 +1106,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1116,12 +1128,35 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="O13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13">
+        <v>6</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="G14" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="P14" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>29</v>
+      </c>
+      <c r="R14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="G15" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Rework debug messages. Build Key exchange finished message
</commit_message>
<xml_diff>
--- a/Protocolo.xlsx
+++ b/Protocolo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmartin\Documents\Arduino\esp-now_mqtt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCC2609-A56F-40C1-8598-8A782C4954A7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E642A6AD-B213-4FA9-A4C4-C5ED82B3CF21}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="13860" windowHeight="5472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>FE</t>
   </si>
   <si>
-    <t>Kslave (16 byte)</t>
-  </si>
-  <si>
     <t>------------------------------------&gt;</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>Server Hello</t>
   </si>
   <si>
-    <t>Kmaster (16 byte)</t>
-  </si>
-  <si>
     <t>Key exchange finished</t>
   </si>
   <si>
@@ -115,6 +109,12 @@
   </si>
   <si>
     <t>Key</t>
+  </si>
+  <si>
+    <t>Kmaster (32 byte)</t>
+  </si>
+  <si>
+    <t>Kslave (32 byte)</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1006,7 @@
   <dimension ref="B2:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1022,7 @@
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
@@ -1035,7 +1035,7 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -1043,95 +1043,95 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2"/>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
         <v>14</v>
       </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" t="s">
         <v>11</v>
-      </c>
-      <c r="J9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
         <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="O13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="P13">
         <v>6</v>
@@ -1145,41 +1145,41 @@
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="G14" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P14" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>27</v>
+      </c>
+      <c r="R14" t="s">
         <v>28</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>29</v>
-      </c>
-      <c r="R14" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" t="s">
         <v>11</v>
-      </c>
-      <c r="K15" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct Random field lengh
</commit_message>
<xml_diff>
--- a/Protocolo.xlsx
+++ b/Protocolo.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmartin\Documents\Arduino\esp-now_mqtt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin_g\Documents\_PRIVATE\Arduino\esp-now_mqtt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E642A6AD-B213-4FA9-A4C4-C5ED82B3CF21}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>FF</t>
   </si>
@@ -51,9 +50,6 @@
     <t>FD</t>
   </si>
   <si>
-    <t>Random (16 byte)</t>
-  </si>
-  <si>
     <t>NodeID (2 byte)</t>
   </si>
   <si>
@@ -115,12 +111,18 @@
   </si>
   <si>
     <t>Kslave (32 byte)</t>
+  </si>
+  <si>
+    <t>Length (2 byte)</t>
+  </si>
+  <si>
+    <t>Random (4 byte)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -720,7 +722,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="Rohde &amp; Schwarz Coloured PrivotTable">
-    <tableStyle name="Rohde &amp; Schwarz Coloured PrivotTable" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Rohde &amp; Schwarz Coloured PrivotTable" table="0" count="10">
       <tableStyleElement type="wholeTable" dxfId="15"/>
       <tableStyleElement type="headerRow" dxfId="14"/>
       <tableStyleElement type="totalRow" dxfId="13"/>
@@ -732,7 +734,7 @@
       <tableStyleElement type="pageFieldLabels" dxfId="7"/>
       <tableStyleElement type="pageFieldValues" dxfId="6"/>
     </tableStyle>
-    <tableStyle name="Rohde &amp; Schwarz Coloured Table" pivot="0" count="6" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="Rohde &amp; Schwarz Coloured Table" pivot="0" count="6">
       <tableStyleElement type="wholeTable" dxfId="5"/>
       <tableStyleElement type="headerRow" dxfId="4"/>
       <tableStyleElement type="totalRow" dxfId="3"/>
@@ -1002,30 +1004,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1033,20 +1035,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>4</v>
@@ -1055,83 +1057,86 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="2"/>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="I9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" t="s">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
         <v>10</v>
       </c>
-      <c r="I9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="O13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P13">
         <v>6</v>
@@ -1143,43 +1148,43 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="G14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>26</v>
+      </c>
+      <c r="R14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
         <v>19</v>
       </c>
-      <c r="P14" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>27</v>
-      </c>
-      <c r="R14" t="s">
-        <v>28</v>
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="G15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="J15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="G18" t="s">
         <v>22</v>
-      </c>
-      <c r="G18" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1189,24 +1194,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update protocol definition doc
</commit_message>
<xml_diff>
--- a/Protocolo.xlsx
+++ b/Protocolo.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>FF</t>
   </si>
@@ -117,6 +117,30 @@
   </si>
   <si>
     <t>Random (4 byte)</t>
+  </si>
+  <si>
+    <t>IV (16 byte)</t>
+  </si>
+  <si>
+    <t>Random 16 Byte</t>
+  </si>
+  <si>
+    <t>IV 16 Byte</t>
+  </si>
+  <si>
+    <t>CRC is generated before encryption and checked after decryption</t>
+  </si>
+  <si>
+    <t>IV is needed to decrypt current packet</t>
+  </si>
+  <si>
+    <t>IV is a 16 byte unencypted random</t>
+  </si>
+  <si>
+    <t>After node receives invalidate key message it should start a key agreement with Client Hello</t>
+  </si>
+  <si>
+    <t>This is answered in case a node trying to send a message is not registered or key is wrong</t>
   </si>
 </sst>
 </file>
@@ -243,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,6 +312,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,10 +476,18 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
@@ -1005,189 +1061,252 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R18"/>
+  <dimension ref="B2:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="11" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+    <row r="4" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="C4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="J4" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="E9" s="1" t="s">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" s="5"/>
+      <c r="I12" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="O13" t="s">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="R13" t="s">
         <v>24</v>
       </c>
-      <c r="P13">
+      <c r="S13">
         <v>6</v>
       </c>
-      <c r="Q13">
+      <c r="T13">
         <v>2</v>
       </c>
-      <c r="R13">
+      <c r="U13">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="G14" s="2" t="s">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="S14" t="s">
+        <v>25</v>
+      </c>
+      <c r="T14" t="s">
+        <v>26</v>
+      </c>
+      <c r="U14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="I18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="P14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>26</v>
-      </c>
-      <c r="R14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="G15" t="s">
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="F19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M19" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" t="s">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="C4:G4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>